<commit_message>
created method that will navigate to any home listing in the us
</commit_message>
<xml_diff>
--- a/com.redfin/src/test/resources/test_data.xlsx
+++ b/com.redfin/src/test/resources/test_data.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.expedia\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.redfin\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBCEEE1-9882-4402-AEA7-514F0B186055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07546DE8-43CF-42E5-8F19-8DFE9791CB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
   <sheets>
     <sheet name="nbaTeams" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="1" r:id="rId2"/>
     <sheet name="bmwModels" sheetId="3" r:id="rId3"/>
     <sheet name="myTrips" sheetId="4" r:id="rId4"/>
+    <sheet name="usaCities" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="121">
   <si>
     <t>City Name</t>
   </si>
@@ -374,6 +375,33 @@
   </si>
   <si>
     <t>Morocco</t>
+  </si>
+  <si>
+    <t>US Cities</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>Tampa</t>
+  </si>
+  <si>
+    <t>Tysons</t>
+  </si>
+  <si>
+    <t>Minneapolis</t>
+  </si>
+  <si>
+    <t>Cincinnati</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>Nashville</t>
+  </si>
+  <si>
+    <t>Seattle</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79F428AD-AE09-447E-9CC1-5B40C17299F3}">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -1343,4 +1371,98 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F168171D-B480-4774-B7A1-6093E7D36237}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
redfin test caes complete (need to fix assertions and work around random pop up)
</commit_message>
<xml_diff>
--- a/com.redfin/src/test/resources/test_data.xlsx
+++ b/com.redfin/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.redfin\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07546DE8-43CF-42E5-8F19-8DFE9791CB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2881D4A-2E21-445A-A216-729CF2973087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
@@ -386,9 +386,6 @@
     <t>Tampa</t>
   </si>
   <si>
-    <t>Tysons</t>
-  </si>
-  <si>
     <t>Minneapolis</t>
   </si>
   <si>
@@ -402,6 +399,9 @@
   </si>
   <si>
     <t>Seattle</t>
+  </si>
+  <si>
+    <t>McLean</t>
   </si>
 </sst>
 </file>
@@ -1377,7 +1377,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F168171D-B480-4774-B7A1-6093E7D36237}">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1403,22 +1405,22 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
@@ -1428,7 +1430,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
@@ -1458,7 +1460,7 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
building custom m series on bmw in progress
</commit_message>
<xml_diff>
--- a/com.redfin/src/test/resources/test_data.xlsx
+++ b/com.redfin/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashar\IdeaProjects\SeleniumBootcampWinterWeekend2022\com.redfin\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2881D4A-2E21-445A-A216-729CF2973087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93D59E3-3F95-4EB3-B1EF-042465DB066A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{7D775343-6CF7-4D85-BA2B-E0C06A58AE89}"/>
   </bookViews>
@@ -1382,6 +1382,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">

</xml_diff>

<commit_message>
Adding 2 more Module TestCases(Redfin, AutomationPractice)
</commit_message>
<xml_diff>
--- a/com.redfin/src/test/resources/test_data.xlsx
+++ b/com.redfin/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malik/IdeaProjects/Team1SeleniumBootcamp/com.redfin/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64D968F-EB04-294E-8BC7-7F7E8D08ABEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C77E285-3060-6044-9423-43F594530E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{7CE48203-893E-5A46-A7A5-5483309E5BAF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>What's New</t>
   </si>
@@ -41,7 +41,85 @@
     <t>Our Dedication to Data Quality</t>
   </si>
   <si>
-    <t>Thanks for signing up for Redfin updates.</t>
+    <t>Search Results for: Virginia</t>
+  </si>
+  <si>
+    <t>Housing Market</t>
+  </si>
+  <si>
+    <t>What is the housing market like right now?</t>
+  </si>
+  <si>
+    <t>22033 Apartments for Rent</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Fairfax</t>
+  </si>
+  <si>
+    <t>San Diego</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>San Antonio</t>
+  </si>
+  <si>
+    <t>Albuquerque</t>
+  </si>
+  <si>
+    <t>New Orleans</t>
+  </si>
+  <si>
+    <t>Wilmington</t>
+  </si>
+  <si>
+    <t>San Francisco</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>Tampa</t>
+  </si>
+  <si>
+    <t>Provo</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Orem</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Nashville</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Boise</t>
   </si>
 </sst>
 </file>
@@ -402,15 +480,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A0FA30F-A4BF-344A-8A71-E5D02DE10FF4}">
-  <dimension ref="A2:A4"/>
+  <dimension ref="A2:A31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="71.6640625" customWidth="1"/>
+    <col min="1" max="1" width="37.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -428,6 +506,141 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added more Redfin TestCases with Assertions
</commit_message>
<xml_diff>
--- a/com.redfin/src/test/resources/test_data.xlsx
+++ b/com.redfin/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malik/IdeaProjects/Team1SeleniumBootcamp/com.redfin/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C77E285-3060-6044-9423-43F594530E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB384B81-EEF5-A445-BC13-C109069B7528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{7CE48203-893E-5A46-A7A5-5483309E5BAF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>What's New</t>
   </si>
@@ -120,6 +120,39 @@
   </si>
   <si>
     <t>Boise</t>
+  </si>
+  <si>
+    <t>Destin</t>
+  </si>
+  <si>
+    <t>Fort Lauderdale</t>
+  </si>
+  <si>
+    <t>Jacksonville</t>
+  </si>
+  <si>
+    <t>Fort Myers</t>
+  </si>
+  <si>
+    <t>Charleston</t>
+  </si>
+  <si>
+    <t>Myrtle Beach</t>
+  </si>
+  <si>
+    <t>Asheville</t>
+  </si>
+  <si>
+    <t>Durham</t>
+  </si>
+  <si>
+    <t>Raleigh</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Louisville</t>
   </si>
 </sst>
 </file>
@@ -480,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A0FA30F-A4BF-344A-8A71-E5D02DE10FF4}">
-  <dimension ref="A2:A31"/>
+  <dimension ref="A2:A42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,6 +674,61 @@
         <v>28</v>
       </c>
     </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding some more Redfin TestCases
</commit_message>
<xml_diff>
--- a/com.redfin/src/test/resources/test_data.xlsx
+++ b/com.redfin/src/test/resources/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malik/IdeaProjects/Team1SeleniumBootcamp/com.redfin/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB384B81-EEF5-A445-BC13-C109069B7528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8474398C-3202-DE4B-8AE9-4FD2F555E936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16520" xr2:uid="{7CE48203-893E-5A46-A7A5-5483309E5BAF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>What's New</t>
   </si>
@@ -153,6 +153,24 @@
   </si>
   <si>
     <t>Louisville</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>Baltimore</t>
+  </si>
+  <si>
+    <t>Milwaukee</t>
+  </si>
+  <si>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>Minneapolis</t>
   </si>
 </sst>
 </file>
@@ -513,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A0FA30F-A4BF-344A-8A71-E5D02DE10FF4}">
-  <dimension ref="A2:A42"/>
+  <dimension ref="A2:A48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -729,6 +747,36 @@
         <v>39</v>
       </c>
     </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>